<commit_message>
Adding the chloropleth map
</commit_message>
<xml_diff>
--- a/country_text.xlsx
+++ b/country_text.xlsx
@@ -1,27 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanna\OneDrive\Documenten\Honours DSEML\EDML\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylene/EDML/Cassowary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3817DCBE-D5B0-4C06-AB54-1D56A1239F30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E656723-15D9-E04D-870F-D8438D9A3835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet0" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet0!$A$1:$B$104</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="22">
   <si>
     <t>country</t>
   </si>
@@ -78,16 +91,32 @@
   </si>
   <si>
     <t>Canada</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>USA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -118,15 +147,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -142,7 +172,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -438,539 +468,625 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A104"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:B104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A83" sqref="A83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="64" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <f>COUNTIF(A2:A104,A2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="B3">
+        <f>COUNTIF(A3:A104,A3)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="B4">
+        <f>COUNTIF(A4:A104,A4)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="B16">
+        <f>COUNTIF(A16:A104,A16)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B21" s="3">
+        <f>COUNTIF(A21:A104,A21)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B22">
+        <f>COUNTIF(A22:A104,A22)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:1" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B31">
+        <f>COUNTIF(A31:A104,A31)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B33">
+        <f>COUNTIF(A33:A104,A33)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B35">
+        <f>COUNTIF(A35:A104,A35)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B40">
+        <f>COUNTIF(A40:A104,A40)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B44">
+        <f>COUNTIF(A44:A104,A44)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+      <c r="B54">
+        <f>COUNTIF(A54:A104,A54)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="62" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:1" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="75" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="79" spans="1:1" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:1" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:1" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="B83">
+        <f>COUNTIF(A83:A104,A83)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B84">
+        <f>COUNTIF(A84:A104,A84)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="91" spans="1:1" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:2" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="95" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B95">
+        <f>COUNTIF(A95:A104,A95)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="B96">
+        <f>COUNTIF(A96:A104,A96)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B97">
+        <f>COUNTIF(A97:A104,A97)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B99">
+        <f>COUNTIF(A99:A104,A99)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:B104" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="1">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1 A104 A95:A103 A90:A94 A81:A89 A80 A4:A79 A2:A3" numberStoredAsText="1"/>
+    <ignoredError sqref="A1 A104 A95:A103 A90:A94 A81:A89 A80 A4:A53 A3 A55:A79" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>